<commit_message>
updated list of Followers from 30.06 (plz make view for this app)
</commit_message>
<xml_diff>
--- a/Followers.xlsx
+++ b/Followers.xlsx
@@ -494,7 +494,7 @@
     <t>7239973909</t>
   </si>
   <si>
-    <t>retchygod</t>
+    <t>24feetofsmoke</t>
   </si>
   <si>
     <t>Ruslan Vadimovich</t>
@@ -1142,7 +1142,7 @@
     <t>n_a_t_a_l_i_94</t>
   </si>
   <si>
-    <t>Наталья</t>
+    <t>Натали</t>
   </si>
   <si>
     <t>45649772571</t>
@@ -1271,6 +1271,15 @@
     <t>Сергей Николаевич</t>
   </si>
   <si>
+    <t>8628968557</t>
+  </si>
+  <si>
+    <t>cybulin2018</t>
+  </si>
+  <si>
+    <t>Сергей Цыбулин</t>
+  </si>
+  <si>
     <t>47540162800</t>
   </si>
   <si>
@@ -1359,15 +1368,6 @@
   </si>
   <si>
     <t>Юляшка (АЛЕКС)</t>
-  </si>
-  <si>
-    <t>47487893687</t>
-  </si>
-  <si>
-    <t>chill.resort</t>
-  </si>
-  <si>
-    <t>𝗖𝗵𝗶𝗹𝗹 𝗥𝗲𝘀𝗼𝗿𝘁💨</t>
   </si>
   <si>
     <t>4390935361</t>

</xml_diff>

<commit_message>
updated list of Followers from 154 to 155 users
</commit_message>
<xml_diff>
--- a/Followers.xlsx
+++ b/Followers.xlsx
@@ -278,6 +278,15 @@
     <t>João Rocha</t>
   </si>
   <si>
+    <t>1289460729</t>
+  </si>
+  <si>
+    <t>miss_kvitka</t>
+  </si>
+  <si>
+    <t>Julia Marushchenko</t>
+  </si>
+  <si>
     <t>7861314594</t>
   </si>
   <si>
@@ -491,148 +500,130 @@
     <t>pupsarin</t>
   </si>
   <si>
+    <t>40924417527</t>
+  </si>
+  <si>
+    <t>sergostruk</t>
+  </si>
+  <si>
+    <t>Serg Ostruk</t>
+  </si>
+  <si>
+    <t>5836516802</t>
+  </si>
+  <si>
+    <t>sixteencolorsofme</t>
+  </si>
+  <si>
+    <t>Sergey Savchenko</t>
+  </si>
+  <si>
+    <t>14019691361</t>
+  </si>
+  <si>
+    <t>sharaman7777</t>
+  </si>
+  <si>
+    <t>Sharaman</t>
+  </si>
+  <si>
+    <t>22591367762</t>
+  </si>
+  <si>
+    <t>oserleoni</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>5480621170</t>
+  </si>
+  <si>
+    <t>steshastepa</t>
+  </si>
+  <si>
+    <t>Stephanie 🌸</t>
+  </si>
+  <si>
+    <t>7404815080</t>
+  </si>
+  <si>
+    <t>kucheryavaya_s</t>
+  </si>
+  <si>
+    <t>Sveta</t>
+  </si>
+  <si>
+    <t>8665544898</t>
+  </si>
+  <si>
+    <t>ser18ab1</t>
+  </si>
+  <si>
+    <t>Table Tennis</t>
+  </si>
+  <si>
+    <t>41902230851</t>
+  </si>
+  <si>
+    <t>timofei.kasianov1992</t>
+  </si>
+  <si>
+    <t>Timofei Kasianov</t>
+  </si>
+  <si>
+    <t>5682107042</t>
+  </si>
+  <si>
+    <t>timurryazantcev</t>
+  </si>
+  <si>
+    <t>Timur Ryazantcev</t>
+  </si>
+  <si>
+    <t>272786242</t>
+  </si>
+  <si>
+    <t>cirius_kh</t>
+  </si>
+  <si>
+    <t>Tolya</t>
+  </si>
+  <si>
+    <t>4448583004</t>
+  </si>
+  <si>
+    <t>shevanton_</t>
+  </si>
+  <si>
+    <t>Toxa</t>
+  </si>
+  <si>
+    <t>3658771700</t>
+  </si>
+  <si>
+    <t>nazar.vita.m</t>
+  </si>
+  <si>
+    <t>Vita</t>
+  </si>
+  <si>
+    <t>5649619609</t>
+  </si>
+  <si>
+    <t>tengoku_</t>
+  </si>
+  <si>
+    <t>Vlada</t>
+  </si>
+  <si>
     <t>7239973909</t>
   </si>
   <si>
-    <t>24feetofsmoke</t>
-  </si>
-  <si>
-    <t>Ruslan Vadimovich</t>
-  </si>
-  <si>
-    <t>1325485215</t>
-  </si>
-  <si>
-    <t>samuel.barreto.357</t>
-  </si>
-  <si>
-    <t>Samuel Barreto</t>
-  </si>
-  <si>
-    <t>40924417527</t>
-  </si>
-  <si>
-    <t>sergostruk</t>
-  </si>
-  <si>
-    <t>Serg Ostruk</t>
-  </si>
-  <si>
-    <t>5836516802</t>
-  </si>
-  <si>
-    <t>sixteencolorsofme</t>
-  </si>
-  <si>
-    <t>Sergey Savchenko</t>
-  </si>
-  <si>
-    <t>14019691361</t>
-  </si>
-  <si>
-    <t>sharaman7777</t>
-  </si>
-  <si>
-    <t>Sharaman</t>
-  </si>
-  <si>
-    <t>22591367762</t>
-  </si>
-  <si>
-    <t>oserleoni</t>
-  </si>
-  <si>
-    <t>SO</t>
-  </si>
-  <si>
-    <t>5480621170</t>
-  </si>
-  <si>
-    <t>steshastepa</t>
-  </si>
-  <si>
-    <t>Stephanie 🌸🌺🌸</t>
-  </si>
-  <si>
-    <t>7404815080</t>
-  </si>
-  <si>
-    <t>kucheryavaya_s</t>
-  </si>
-  <si>
-    <t>Sveta</t>
-  </si>
-  <si>
-    <t>8665544898</t>
-  </si>
-  <si>
-    <t>ser18ab1</t>
-  </si>
-  <si>
-    <t>Table Tennis</t>
-  </si>
-  <si>
-    <t>41902230851</t>
-  </si>
-  <si>
-    <t>timofei.kasianov1992</t>
-  </si>
-  <si>
-    <t>Timofei Kasianov</t>
-  </si>
-  <si>
-    <t>5682107042</t>
-  </si>
-  <si>
-    <t>timurryazantcev</t>
-  </si>
-  <si>
-    <t>Timur Ryazantcev</t>
-  </si>
-  <si>
-    <t>272786242</t>
-  </si>
-  <si>
-    <t>cirius_kh</t>
-  </si>
-  <si>
-    <t>Tolya</t>
-  </si>
-  <si>
-    <t>4448583004</t>
-  </si>
-  <si>
-    <t>shevanton_</t>
-  </si>
-  <si>
-    <t>Toxa</t>
-  </si>
-  <si>
-    <t>3658771700</t>
-  </si>
-  <si>
-    <t>nazar.vita.m</t>
-  </si>
-  <si>
-    <t>Vita</t>
-  </si>
-  <si>
-    <t>5649619609</t>
-  </si>
-  <si>
-    <t>tengoku_</t>
-  </si>
-  <si>
-    <t>Vlada</t>
-  </si>
-  <si>
-    <t>1289460729</t>
-  </si>
-  <si>
-    <t>miss_kvitka</t>
-  </si>
-  <si>
-    <t>Yulia</t>
+    <t>piuumee</t>
+  </si>
+  <si>
+    <t>ʀᴜꜱʟᴀɴ ᴠᴀᴅɪᴍᴏᴠɪᴄʜ</t>
   </si>
   <si>
     <t>2460313075</t>
@@ -845,7 +836,7 @@
     <t>vova_mixx</t>
   </si>
   <si>
-    <t>Вова Сериков</t>
+    <t>Владимир Сериков</t>
   </si>
   <si>
     <t>17617023602</t>
@@ -963,6 +954,15 @@
   </si>
   <si>
     <t>Иван Безменов</t>
+  </si>
+  <si>
+    <t>39408861207</t>
+  </si>
+  <si>
+    <t>ivanvinnikov_06</t>
+  </si>
+  <si>
+    <t>Иван Винников</t>
   </si>
   <si>
     <t>39383552563</t>
@@ -2038,15 +2038,15 @@
         <v>158</v>
       </c>
       <c r="C55" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C56" t="s">
         <v>161</v>
@@ -2291,18 +2291,18 @@
         <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>227</v>
+      </c>
+      <c r="B79" t="s">
         <v>228</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>229</v>
-      </c>
-      <c r="C79" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="80">

</xml_diff>

<commit_message>
updated list of Followers from 155 to 162 users
</commit_message>
<xml_diff>
--- a/Followers.xlsx
+++ b/Followers.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="479">
   <si>
     <t>1665158140</t>
   </si>
@@ -92,7 +92,7 @@
     <t>22927148540</t>
   </si>
   <si>
-    <t>utepilsrame</t>
+    <t>senorita_anastasita</t>
   </si>
   <si>
     <t>Anastasia</t>
@@ -197,6 +197,24 @@
     <t>Dmitry Smirnov</t>
   </si>
   <si>
+    <t>47870145431</t>
+  </si>
+  <si>
+    <t>dr.tabletennis</t>
+  </si>
+  <si>
+    <t>Dr. Table Tennis</t>
+  </si>
+  <si>
+    <t>37337003520</t>
+  </si>
+  <si>
+    <t>apextech.co</t>
+  </si>
+  <si>
+    <t>Driven by Synergy</t>
+  </si>
+  <si>
     <t>5653354215</t>
   </si>
   <si>
@@ -341,6 +359,15 @@
     <t>Kyryl Vasylenko</t>
   </si>
   <si>
+    <t>38430788275</t>
+  </si>
+  <si>
+    <t>latte_lancey_</t>
+  </si>
+  <si>
+    <t>Lancey  Latte</t>
+  </si>
+  <si>
     <t>5978809531</t>
   </si>
   <si>
@@ -350,6 +377,15 @@
     <t>Lena</t>
   </si>
   <si>
+    <t>1499488855</t>
+  </si>
+  <si>
+    <t>listo717</t>
+  </si>
+  <si>
+    <t>Listowellagyemang</t>
+  </si>
+  <si>
     <t>5589026095</t>
   </si>
   <si>
@@ -377,6 +413,15 @@
     <t>Locenok</t>
   </si>
   <si>
+    <t>1080866431</t>
+  </si>
+  <si>
+    <t>manuel_kobbi</t>
+  </si>
+  <si>
+    <t>Manuel Kobby</t>
+  </si>
+  <si>
     <t>4974294280</t>
   </si>
   <si>
@@ -485,6 +530,15 @@
     <t>Olha Sanzharovska</t>
   </si>
   <si>
+    <t>4872254528</t>
+  </si>
+  <si>
+    <t>podarki_podarki_podarki</t>
+  </si>
+  <si>
+    <t>Podarki Podarki</t>
+  </si>
+  <si>
     <t>6720001536</t>
   </si>
   <si>
@@ -500,6 +554,15 @@
     <t>pupsarin</t>
   </si>
   <si>
+    <t>7239973909</t>
+  </si>
+  <si>
+    <t>piuumee</t>
+  </si>
+  <si>
+    <t>Ruslan Vadimovich</t>
+  </si>
+  <si>
     <t>40924417527</t>
   </si>
   <si>
@@ -617,15 +680,6 @@
     <t>Vlada</t>
   </si>
   <si>
-    <t>7239973909</t>
-  </si>
-  <si>
-    <t>piuumee</t>
-  </si>
-  <si>
-    <t>ʀᴜꜱʟᴀɴ ᴠᴀᴅɪᴍᴏᴠɪᴄʜ</t>
-  </si>
-  <si>
     <t>2460313075</t>
   </si>
   <si>
@@ -875,6 +929,15 @@
     <t>Даша Луцива</t>
   </si>
   <si>
+    <t>8344571483</t>
+  </si>
+  <si>
+    <t>ibragimov_jal</t>
+  </si>
+  <si>
+    <t>Джалиль Ибрагимов</t>
+  </si>
+  <si>
     <t>6972153229</t>
   </si>
   <si>
@@ -989,7 +1052,7 @@
     <t>katiushakhomut</t>
   </si>
   <si>
-    <t>Катюшка 🎀 Хомут</t>
+    <t>Катюша Хомут</t>
   </si>
   <si>
     <t>1507437372</t>
@@ -1190,6 +1253,15 @@
     <t>Олег Баранов</t>
   </si>
   <si>
+    <t>9365290165</t>
+  </si>
+  <si>
+    <t>olegavrishenko</t>
+  </si>
+  <si>
+    <t>Олег Гавришенко</t>
+  </si>
+  <si>
     <t>9295779044</t>
   </si>
   <si>
@@ -1307,15 +1379,6 @@
     <t>СТУДИЯ JJ</t>
   </si>
   <si>
-    <t>4872254528</t>
-  </si>
-  <si>
-    <t>tanya_tanyushka_podarki</t>
-  </si>
-  <si>
-    <t>Татьяна Павлова</t>
-  </si>
-  <si>
     <t>9375328733</t>
   </si>
   <si>
@@ -1373,7 +1436,7 @@
     <t>4390935361</t>
   </si>
   <si>
-    <t>olhapozyvailo</t>
+    <t>olyapozyvailo</t>
   </si>
   <si>
     <t>𝙾𝚕𝚑𝚊 𝙿𝚘𝚣𝚢𝚟𝚊𝚒𝚕𝚘</t>
@@ -1430,7 +1493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C155"/>
+  <dimension ref="A1:C162"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2049,70 +2112,70 @@
         <v>161</v>
       </c>
       <c r="C56" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B58" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B59" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C59" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B60" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C60" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B61" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C61" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B62" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C62" t="s">
         <v>179</v>
@@ -2291,73 +2354,73 @@
         <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B79" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C79" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B80" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C80" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B81" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C81" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B82" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C82" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B83" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C83" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
+        <v>243</v>
+      </c>
+      <c r="B84" t="s">
+        <v>244</v>
+      </c>
+      <c r="C84" t="s">
         <v>242</v>
-      </c>
-      <c r="B84" t="s">
-        <v>243</v>
-      </c>
-      <c r="C84" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="85">
@@ -3139,6 +3202,83 @@
       </c>
       <c r="C155" t="s">
         <v>457</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>458</v>
+      </c>
+      <c r="B156" t="s">
+        <v>459</v>
+      </c>
+      <c r="C156" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>461</v>
+      </c>
+      <c r="B157" t="s">
+        <v>462</v>
+      </c>
+      <c r="C157" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>464</v>
+      </c>
+      <c r="B158" t="s">
+        <v>465</v>
+      </c>
+      <c r="C158" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>467</v>
+      </c>
+      <c r="B159" t="s">
+        <v>468</v>
+      </c>
+      <c r="C159" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>470</v>
+      </c>
+      <c r="B160" t="s">
+        <v>471</v>
+      </c>
+      <c r="C160" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>473</v>
+      </c>
+      <c r="B161" t="s">
+        <v>474</v>
+      </c>
+      <c r="C161" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>476</v>
+      </c>
+      <c r="B162" t="s">
+        <v>477</v>
+      </c>
+      <c r="C162" t="s">
+        <v>478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>